<commit_message>
Actualización automática 2025-05-28 17:15:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>2266.66</v>
       </c>
     </row>
     <row r="14">
@@ -2467,7 +2467,7 @@
         <v>1352.8</v>
       </c>
       <c r="F27" s="6" t="n">
-        <v>7768.719999999999</v>
+        <v>10035.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-28 17:20:07
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>2266.66</v>
+        <v>3122.02</v>
       </c>
     </row>
     <row r="14">
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>5354.86</v>
+        <v>6725.74</v>
       </c>
     </row>
     <row r="18">
@@ -2467,7 +2467,7 @@
         <v>1352.8</v>
       </c>
       <c r="F27" s="6" t="n">
-        <v>10035.38</v>
+        <v>12261.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-29 08:40:07
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -927,7 +927,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
+          <t>DISALME CIA. LTDA.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -975,7 +975,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
+          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GRANIMUNDO S.A.</t>
+          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LINO TUMBACO VICENTE JAVIER</t>
+          <t>GRANIMUNDO S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
+          <t>LINO TUMBACO VICENTE JAVIER</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
+          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>226.8</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
         <v>0</v>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
+          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0</v>
+        <v>226.8</v>
       </c>
       <c r="M16" s="2" t="n">
         <v>0</v>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PAREDES ORTIZ MARIA INES</t>
+          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1311,14 +1311,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RENOVA&amp;DISEÑA S.A.</t>
+          <t>PAREDES ORTIZ MARIA INES</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>91.58</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0</v>
@@ -1339,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>921.02</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>113.4</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2" t="n">
         <v>0</v>
@@ -1359,14 +1359,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>REYES AGUILERA JESSICA ELIZABETH</t>
+          <t>RENOVA&amp;DISEÑA S.A.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>91.58</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0</v>
@@ -1387,10 +1387,10 @@
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>0</v>
+        <v>921.02</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>0</v>
+        <v>113.4</v>
       </c>
       <c r="M19" s="2" t="n">
         <v>0</v>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ROCA REYNA PAUL DAVID</t>
+          <t>REYES AGUILERA JESSICA ELIZABETH</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>ROCA REYNA PAUL DAVID</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -1695,105 +1695,153 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="D27" s="4" t="inlineStr">
-        <is>
-          <t>1 de 25</t>
-        </is>
-      </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="F27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="G27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="H27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="I27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="J27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="K27" s="4" t="inlineStr">
-        <is>
-          <t>1 de 25</t>
-        </is>
-      </c>
-      <c r="L27" s="4" t="inlineStr">
-        <is>
-          <t>2 de 25</t>
-        </is>
-      </c>
-      <c r="M27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
-        </is>
-      </c>
-      <c r="N27" s="4" t="inlineStr">
-        <is>
-          <t>0 de 25</t>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="D28" s="4" t="inlineStr">
+        <is>
+          <t>1 de 26</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="F28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="H28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="I28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="J28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="K28" s="4" t="inlineStr">
+        <is>
+          <t>1 de 26</t>
+        </is>
+      </c>
+      <c r="L28" s="4" t="inlineStr">
+        <is>
+          <t>2 de 26</t>
+        </is>
+      </c>
+      <c r="M28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
+        </is>
+      </c>
+      <c r="N28" s="4" t="inlineStr">
+        <is>
+          <t>0 de 26</t>
         </is>
       </c>
     </row>
@@ -1808,7 +1856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2056,7 +2104,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
+          <t>DISALME CIA. LTDA.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -2080,7 +2128,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
+          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -2104,7 +2152,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GRANIMUNDO S.A.</t>
+          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -2128,20 +2176,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LINO TUMBACO VICENTE JAVIER</t>
+          <t>GRANIMUNDO S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>1444.13</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>3122.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2152,20 +2200,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
+          <t>LINO TUMBACO VICENTE JAVIER</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>1444.13</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0</v>
+        <v>3122.02</v>
       </c>
     </row>
     <row r="15">
@@ -2176,7 +2224,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
+          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -2186,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>226.8</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2248,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
+          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -2210,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0</v>
+        <v>226.8</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
@@ -2224,7 +2272,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PAREDES ORTIZ MARIA INES</t>
+          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -2237,7 +2285,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>6725.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2248,20 +2296,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RENOVA&amp;DISEÑA S.A.</t>
+          <t>PAREDES ORTIZ MARIA INES</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>683.0700000000001</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>800.79</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>1126</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>6725.74</v>
       </c>
     </row>
     <row r="19">
@@ -2272,17 +2320,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>REYES AGUILERA JESSICA ELIZABETH</t>
+          <t>RENOVA&amp;DISEÑA S.A.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0</v>
+        <v>683.0700000000001</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>800.79</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0</v>
+        <v>1126</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
@@ -2296,20 +2344,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ROCA REYNA PAUL DAVID</t>
+          <t>REYES AGUILERA JESSICA ELIZABETH</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>1914.22</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>738.55</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>1994.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2320,20 +2368,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>ROCA REYNA PAUL DAVID</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0</v>
+        <v>1914.22</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0</v>
+        <v>738.55</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0</v>
+        <v>1994.73</v>
       </c>
     </row>
     <row r="22">
@@ -2344,7 +2392,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -2368,7 +2416,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -2392,7 +2440,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -2416,11 +2464,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>1739.16</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>0</v>
@@ -2440,33 +2488,57 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>1739.16</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" s="6" t="n">
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="6" t="n">
         <v>5276.07</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D28" s="6" t="n">
         <v>2983.47</v>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E28" s="6" t="n">
         <v>1352.8</v>
       </c>
-      <c r="F27" s="6" t="n">
+      <c r="F28" s="6" t="n">
         <v>12261.62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-05-29 09:15:07
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1503,7 +1503,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -1743,105 +1743,153 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="D28" s="4" t="inlineStr">
-        <is>
-          <t>1 de 26</t>
-        </is>
-      </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="F28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="G28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="H28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="I28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="J28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="K28" s="4" t="inlineStr">
-        <is>
-          <t>1 de 26</t>
-        </is>
-      </c>
-      <c r="L28" s="4" t="inlineStr">
-        <is>
-          <t>2 de 26</t>
-        </is>
-      </c>
-      <c r="M28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="N28" s="4" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="D29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="F29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="H29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="I29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="J29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="K29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="L29" s="4" t="inlineStr">
+        <is>
+          <t>2 de 27</t>
+        </is>
+      </c>
+      <c r="M29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="N29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2392,7 +2440,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -2416,7 +2464,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -2440,7 +2488,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -2464,7 +2512,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2488,11 +2536,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>1739.16</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>0</v>
@@ -2512,33 +2560,57 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>1739.16</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" s="6" t="n">
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="6" t="n">
         <v>5276.07</v>
       </c>
-      <c r="D28" s="6" t="n">
+      <c r="D29" s="6" t="n">
         <v>2983.47</v>
       </c>
-      <c r="E28" s="6" t="n">
+      <c r="E29" s="6" t="n">
         <v>1352.8</v>
       </c>
-      <c r="F28" s="6" t="n">
+      <c r="F29" s="6" t="n">
         <v>12261.62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-12 17:20:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -2732,7 +2732,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2806,13 +2806,13 @@
         <v>3120.1145</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>274.75</v>
+        <v>1778.11</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2845.3645</v>
+        <v>1342.0045</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.08805766583245582</v>
+        <v>0.5698861371914395</v>
       </c>
     </row>
     <row r="4">
@@ -3094,13 +3094,13 @@
         <v>1638</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>1753.96</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1638</v>
+        <v>-115.96</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>1.070793650793651</v>
       </c>
     </row>
     <row r="16">
@@ -3185,13 +3185,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>6277.42</v>
+        <v>9534.74</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>17222.58093005039</v>
+        <v>13965.26093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2671242447472763</v>
+        <v>0.4057336009637152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-12 17:25:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -2806,13 +2806,13 @@
         <v>3120.1145</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1778.11</v>
+        <v>1869.69</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>1342.0045</v>
+        <v>1250.4245</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.5698861371914395</v>
+        <v>0.5992376241320631</v>
       </c>
     </row>
     <row r="4">
@@ -3185,13 +3185,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>9534.74</v>
+        <v>9626.32</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>13965.26093005039</v>
+        <v>13873.68093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4057336009637152</v>
+        <v>0.40963062208608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-16 17:10:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>0</v>
+        <v>1108.6</v>
       </c>
       <c r="M21" s="2" t="n">
         <v>0</v>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="L29" s="4" t="inlineStr">
         <is>
-          <t>0 de 27</t>
+          <t>1 de 27</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -2864,7 +2864,7 @@
         <v>1994.73</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>2116.73</v>
+        <v>3225.33</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>2000</v>
@@ -3070,7 +3070,7 @@
         <v>12261.62</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>3038.56</v>
+        <v>4147.16</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>20500</v>
@@ -3462,13 +3462,13 @@
         <v>1638</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>1753.96</v>
+        <v>2862.56</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-115.96</v>
+        <v>-1224.56</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>1.070793650793651</v>
+        <v>1.747594627594627</v>
       </c>
     </row>
     <row r="16">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>9626.32</v>
+        <v>10734.92</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>13873.68093005039</v>
+        <v>12765.08093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.40963062208608</v>
+        <v>0.4568050883041809</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-18 13:35:10
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1598,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>183.17</v>
+        <v>366.34</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0</v>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>183.17</v>
+        <v>366.34</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>1000</v>
@@ -3070,7 +3070,7 @@
         <v>12261.62</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>6118.24</v>
+        <v>6301.41</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>20500</v>
@@ -3174,13 +3174,13 @@
         <v>3120.1145</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2344.89</v>
+        <v>2528.06</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>775.2245000000003</v>
+        <v>592.0545000000002</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.7515397271478338</v>
+        <v>0.8102459060396662</v>
       </c>
     </row>
     <row r="4">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>12506.69</v>
+        <v>12689.86</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>10993.31093005039</v>
+        <v>10810.14093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5321995534054297</v>
+        <v>0.5399940211820574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-19 15:30:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -3438,13 +3438,13 @@
         <v>483</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>629.48</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>483</v>
+        <v>-146.48</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0</v>
+        <v>1.303271221532091</v>
       </c>
     </row>
     <row r="15">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>12689.86</v>
+        <v>13319.34</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>10810.14093005039</v>
+        <v>10180.66093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5399940211820574</v>
+        <v>0.5667804031006666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 13:10:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1475,13 +1475,13 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>648</v>
+        <v>2851.2</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>475.2</v>
+        <v>1742.4</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0</v>
+        <v>730.35</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>0</v>
+        <v>2691.25</v>
       </c>
       <c r="M17" s="2" t="n">
         <v>774.7</v>
@@ -2196,42 +2196,42 @@
       </c>
       <c r="E29" s="4" t="inlineStr">
         <is>
+          <t>2 de 27</t>
+        </is>
+      </c>
+      <c r="F29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="inlineStr">
+        <is>
           <t>1 de 27</t>
         </is>
       </c>
-      <c r="F29" s="4" t="inlineStr">
+      <c r="H29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="G29" s="4" t="inlineStr">
+      <c r="I29" s="4" t="inlineStr">
         <is>
           <t>1 de 27</t>
         </is>
       </c>
-      <c r="H29" s="4" t="inlineStr">
+      <c r="J29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="I29" s="4" t="inlineStr">
-        <is>
-          <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="J29" s="4" t="inlineStr">
+      <c r="K29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="K29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
       <c r="L29" s="4" t="inlineStr">
         <is>
-          <t>1 de 27</t>
+          <t>2 de 27</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>1971.08</v>
+        <v>8863.08</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>3000</v>
@@ -3070,7 +3070,7 @@
         <v>12261.62</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>6301.41</v>
+        <v>13193.41</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>20500</v>
@@ -3150,13 +3150,13 @@
         <v>344.284604629486</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>648</v>
+        <v>2851.2</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-303.715395370514</v>
+        <v>-2506.915395370514</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>1.882163742690057</v>
+        <v>8.281520467836252</v>
       </c>
     </row>
     <row r="3">
@@ -3174,13 +3174,13 @@
         <v>3120.1145</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2528.06</v>
+        <v>3795.26</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>592.0545000000002</v>
+        <v>-675.1455000000001</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.8102459060396662</v>
+        <v>1.216384847415055</v>
       </c>
     </row>
     <row r="4">
@@ -3198,13 +3198,13 @@
         <v>250.631825420901</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1207.11</v>
+        <v>1937.46</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-956.4781745790989</v>
+        <v>-1686.828174579099</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>4.81626783818387</v>
+        <v>7.730303191728774</v>
       </c>
     </row>
     <row r="5">
@@ -3462,13 +3462,13 @@
         <v>1638</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>2862.56</v>
+        <v>5553.81</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-1224.56</v>
+        <v>-3915.81</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>1.747594627594627</v>
+        <v>3.390604395604396</v>
       </c>
     </row>
     <row r="16">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>13319.34</v>
+        <v>20211.34</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>10180.66093005039</v>
+        <v>3288.660930050386</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5667804031006666</v>
+        <v>0.8600569872384538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 13:20:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1475,7 +1475,7 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>2851.2</v>
+        <v>3473.28</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>1742.4</v>
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>8863.08</v>
+        <v>9485.16</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>3000</v>
@@ -3070,7 +3070,7 @@
         <v>12261.62</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>13193.41</v>
+        <v>13815.49</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>20500</v>
@@ -3150,13 +3150,13 @@
         <v>344.284604629486</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2851.2</v>
+        <v>3473.28</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-2506.915395370514</v>
+        <v>-3128.995395370514</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>8.281520467836252</v>
+        <v>10.08839766081871</v>
       </c>
     </row>
     <row r="3">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>20211.34</v>
+        <v>20833.42</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>3288.660930050386</v>
+        <v>2666.580930050387</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.8600569872384538</v>
+        <v>0.8865284755525042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 13:35:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1490,7 +1490,7 @@
         <v>36.63</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>0</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>36.55</v>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="H29" s="4" t="inlineStr">
         <is>
-          <t>0 de 27</t>
+          <t>1 de 27</t>
         </is>
       </c>
       <c r="I29" s="4" t="inlineStr">
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>9485.16</v>
+        <v>9556.26</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>3000</v>
@@ -3070,7 +3070,7 @@
         <v>12261.62</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>13815.49</v>
+        <v>13886.59</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>20500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 16:00:10
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1625,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0</v>
+        <v>45.36</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>0</v>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="M29" s="4" t="inlineStr">
         <is>
-          <t>1 de 27</t>
+          <t>2 de 27</t>
         </is>
       </c>
       <c r="N29" s="4" t="inlineStr">
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>366.34</v>
+        <v>411.7</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>1000</v>
@@ -3070,7 +3070,7 @@
         <v>12261.62</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>13886.59</v>
+        <v>13931.95</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>20500</v>
@@ -3486,13 +3486,13 @@
         <v>13061.58</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>3327.4</v>
+        <v>3372.76</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>9734.18</v>
+        <v>9688.82</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2547471286015934</v>
+        <v>0.2582199090768498</v>
       </c>
     </row>
     <row r="17">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>20833.42</v>
+        <v>20878.78</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>2666.580930050387</v>
+        <v>2621.220930050386</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.8865284755525042</v>
+        <v>0.8884586882420704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 16:20:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -3174,13 +3174,13 @@
         <v>3120.1145</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3795.26</v>
+        <v>4080.38</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-675.1455000000001</v>
+        <v>-960.2655</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>1.216384847415055</v>
+        <v>1.307766109224517</v>
       </c>
     </row>
     <row r="4">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>20878.78</v>
+        <v>21163.9</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>2621.220930050386</v>
+        <v>2336.100930050386</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.8884586882420704</v>
+        <v>0.9005914537193432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-30 15:05:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0</v>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>0</v>
+        <v>762.16</v>
       </c>
       <c r="O14" s="2" t="n">
         <v>0</v>
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>0</v>
+        <v>646.75</v>
       </c>
       <c r="R14" s="2" t="n">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
@@ -2196,67 +2196,67 @@
       </c>
       <c r="E29" s="4" t="inlineStr">
         <is>
+          <t>4 de 27</t>
+        </is>
+      </c>
+      <c r="F29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="H29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="I29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="J29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="K29" s="4" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="L29" s="4" t="inlineStr">
+        <is>
           <t>2 de 27</t>
         </is>
       </c>
-      <c r="F29" s="4" t="inlineStr">
+      <c r="M29" s="4" t="inlineStr">
+        <is>
+          <t>2 de 27</t>
+        </is>
+      </c>
+      <c r="N29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="O29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="P29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="G29" s="4" t="inlineStr">
+      <c r="Q29" s="4" t="inlineStr">
         <is>
           <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="H29" s="4" t="inlineStr">
-        <is>
-          <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="I29" s="4" t="inlineStr">
-        <is>
-          <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="J29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="K29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="L29" s="4" t="inlineStr">
-        <is>
-          <t>2 de 27</t>
-        </is>
-      </c>
-      <c r="M29" s="4" t="inlineStr">
-        <is>
-          <t>2 de 27</t>
-        </is>
-      </c>
-      <c r="N29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="O29" s="4" t="inlineStr">
-        <is>
-          <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="P29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="Q29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
         </is>
       </c>
       <c r="R29" s="4" t="inlineStr">
@@ -2675,7 +2675,7 @@
         <v>3122.02</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0</v>
+        <v>1473.73</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>2500</v>
@@ -2783,7 +2783,7 @@
         <v>6725.74</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>3000</v>
@@ -3070,7 +3070,7 @@
         <v>12261.62</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>13931.95</v>
+        <v>15470.5</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>20500</v>
@@ -3198,13 +3198,13 @@
         <v>250.631825420901</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1937.46</v>
+        <v>2067.1</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-1686.828174579099</v>
+        <v>-1816.468174579099</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>7.730303191728774</v>
+        <v>8.247555937992294</v>
       </c>
     </row>
     <row r="5">
@@ -3438,13 +3438,13 @@
         <v>483</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>629.48</v>
+        <v>1276.23</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>-146.48</v>
+        <v>-793.23</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>1.303271221532091</v>
+        <v>2.642298136645963</v>
       </c>
     </row>
     <row r="15">
@@ -3510,13 +3510,13 @@
         <v>342</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>762.16</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>342</v>
+        <v>-420.16</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>2.228538011695906</v>
       </c>
     </row>
     <row r="18">
@@ -3553,13 +3553,13 @@
         <v>23500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>21163.9</v>
+        <v>22702.45</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>2336.100930050386</v>
+        <v>797.5509300503857</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.9005914537193432</v>
+        <v>0.9660616638942116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-03 15:45:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>0</v>
+        <v>2177.28</v>
       </c>
       <c r="N18" s="2" t="n">
         <v>0</v>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="M29" s="4" t="inlineStr">
         <is>
-          <t>0 de 27</t>
+          <t>1 de 27</t>
         </is>
       </c>
       <c r="N29" s="4" t="inlineStr">
@@ -2289,7 +2289,7 @@
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2783,7 +2783,7 @@
         <v>64.81999999999999</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>2177.28</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>6000</v>
@@ -3070,7 +3070,7 @@
         <v>15470.5</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>0</v>
+        <v>2177.28</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>23500</v>
@@ -3098,9 +3098,9 @@
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3486,13 +3486,13 @@
         <v>17085.89</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0</v>
+        <v>2177.28</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>17085.89</v>
+        <v>14908.61</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0</v>
+        <v>0.1274314653787424</v>
       </c>
     </row>
     <row r="17">
@@ -3553,13 +3553,13 @@
         <v>27181.31093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>2177.28</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>27181.31093005039</v>
+        <v>25004.03093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0</v>
+        <v>0.08010209682686427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-14 09:30:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1622,10 +1622,10 @@
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>0</v>
+        <v>309.47</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0</v>
+        <v>1735.84</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>0</v>
@@ -2231,12 +2231,12 @@
       </c>
       <c r="L29" s="4" t="inlineStr">
         <is>
-          <t>0 de 27</t>
+          <t>1 de 27</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
         <is>
-          <t>1 de 27</t>
+          <t>2 de 27</t>
         </is>
       </c>
       <c r="N29" s="4" t="inlineStr">
@@ -2810,7 +2810,7 @@
         <v>411.7</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>2045.31</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>2000</v>
@@ -3070,7 +3070,7 @@
         <v>15470.5</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>1618.96</v>
+        <v>3664.27</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>23500</v>
@@ -3462,13 +3462,13 @@
         <v>1638</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>309.47</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1638</v>
+        <v>1328.53</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>0.1889316239316239</v>
       </c>
     </row>
     <row r="16">
@@ -3486,13 +3486,13 @@
         <v>17085.89</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2177.28</v>
+        <v>3913.12</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>14908.61</v>
+        <v>13172.77</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1274314653787424</v>
+        <v>0.2290264071698928</v>
       </c>
     </row>
     <row r="17">
@@ -3553,13 +3553,13 @@
         <v>27181.31093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1618.96</v>
+        <v>3664.27</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>25562.35093005039</v>
+        <v>23517.04093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.05956151284116889</v>
+        <v>0.1348084354514688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-17 17:25:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -3510,13 +3510,13 @@
         <v>342</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>-513.72</v>
+        <v>-279.25</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>855.72</v>
+        <v>621.25</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>-1.502105263157895</v>
+        <v>-0.8165204678362573</v>
       </c>
     </row>
     <row r="18">
@@ -3553,13 +3553,13 @@
         <v>27181.31093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3664.27</v>
+        <v>3898.74</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>23517.04093005039</v>
+        <v>23282.57093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1348084354514688</v>
+        <v>0.143434583049846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-22 17:15:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>0</v>
+        <v>565.25</v>
       </c>
       <c r="M14" s="2" t="n">
         <v>0</v>
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0</v>
+        <v>1900.8</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0</v>
@@ -2191,47 +2191,47 @@
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="E29" s="4" t="inlineStr">
+      <c r="F29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="F29" s="4" t="inlineStr">
+      <c r="G29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="G29" s="4" t="inlineStr">
+      <c r="H29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="H29" s="4" t="inlineStr">
+      <c r="I29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="I29" s="4" t="inlineStr">
+      <c r="J29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="J29" s="4" t="inlineStr">
+      <c r="K29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="K29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
       <c r="L29" s="4" t="inlineStr">
         <is>
-          <t>1 de 27</t>
+          <t>2 de 27</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -2675,7 +2675,7 @@
         <v>1473.73</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>-558.3200000000001</v>
+        <v>6.93</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>2500</v>
@@ -2783,7 +2783,7 @@
         <v>64.81999999999999</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>2177.28</v>
+        <v>4078.08</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>6000</v>
@@ -3070,7 +3070,7 @@
         <v>15470.5</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>3664.27</v>
+        <v>6130.32</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>23500</v>
@@ -3174,13 +3174,13 @@
         <v>3120.1145</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>1900.8</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>3120.1145</v>
+        <v>1219.3145</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.6092084120630828</v>
       </c>
     </row>
     <row r="4">
@@ -3462,13 +3462,13 @@
         <v>1638</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>309.47</v>
+        <v>874.72</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1328.53</v>
+        <v>763.28</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.1889316239316239</v>
+        <v>0.5340170940170941</v>
       </c>
     </row>
     <row r="16">
@@ -3553,13 +3553,13 @@
         <v>27181.31093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3898.74</v>
+        <v>6364.79</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>23282.57093005039</v>
+        <v>20816.52093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.143434583049846</v>
+        <v>0.2341605236178431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-22 17:20:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>1900.8</v>
+        <v>6514.56</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0</v>
@@ -2783,7 +2783,7 @@
         <v>64.81999999999999</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>4078.08</v>
+        <v>8691.84</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>6000</v>
@@ -3070,7 +3070,7 @@
         <v>15470.5</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>6130.32</v>
+        <v>10744.08</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>23500</v>
@@ -3174,13 +3174,13 @@
         <v>3120.1145</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1900.8</v>
+        <v>6514.56</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>1219.3145</v>
+        <v>-3394.4455</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.6092084120630828</v>
+        <v>2.08792337588893</v>
       </c>
     </row>
     <row r="4">
@@ -3553,13 +3553,13 @@
         <v>27181.31093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>6364.79</v>
+        <v>10978.55</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>20816.52093005039</v>
+        <v>16202.76093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2341605236178431</v>
+        <v>0.4039006811795317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-30 08:30:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
+        <v>250.56</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
@@ -1322,10 +1322,10 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>565.25</v>
+        <v>3217</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0</v>
+        <v>1081.17</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>-513.72</v>
@@ -2186,49 +2186,49 @@
     <row r="29">
       <c r="C29" s="4" t="inlineStr">
         <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="D29" s="4" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="D29" s="4" t="inlineStr">
-        <is>
-          <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="E29" s="4" t="inlineStr">
+      <c r="F29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="F29" s="4" t="inlineStr">
+      <c r="G29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="G29" s="4" t="inlineStr">
+      <c r="H29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="H29" s="4" t="inlineStr">
+      <c r="I29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="I29" s="4" t="inlineStr">
+      <c r="J29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="J29" s="4" t="inlineStr">
+      <c r="K29" s="4" t="inlineStr">
         <is>
           <t>0 de 27</t>
         </is>
       </c>
-      <c r="K29" s="4" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
       <c r="L29" s="4" t="inlineStr">
         <is>
           <t>2 de 27</t>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="M29" s="4" t="inlineStr">
         <is>
-          <t>2 de 27</t>
+          <t>3 de 27</t>
         </is>
       </c>
       <c r="N29" s="4" t="inlineStr">
@@ -2675,7 +2675,7 @@
         <v>1473.73</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>6.93</v>
+        <v>3990.41</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>2500</v>
@@ -3070,7 +3070,7 @@
         <v>15470.5</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>10744.08</v>
+        <v>14727.56</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>23500</v>
@@ -3099,7 +3099,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -3150,13 +3150,13 @@
         <v>344.284604629486</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>250.56</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>344.284604629486</v>
+        <v>93.72460462948601</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0</v>
+        <v>0.7277699805068222</v>
       </c>
     </row>
     <row r="3">
@@ -3462,13 +3462,13 @@
         <v>1638</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>874.72</v>
+        <v>3526.47</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>763.28</v>
+        <v>-1888.47</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.5340170940170941</v>
+        <v>2.152912087912088</v>
       </c>
     </row>
     <row r="16">
@@ -3486,13 +3486,13 @@
         <v>17085.89</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>3913.12</v>
+        <v>4994.29</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>13172.77</v>
+        <v>12091.6</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2290264071698928</v>
+        <v>0.2923049369977215</v>
       </c>
     </row>
     <row r="17">
@@ -3553,13 +3553,13 @@
         <v>27181.31093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>10978.55</v>
+        <v>14962.03</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>16202.76093005039</v>
+        <v>12219.28093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4039006811795317</v>
+        <v>0.5504528474915711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-08 16:15:10
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1625,7 +1625,7 @@
         <v>1670.43</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0</v>
+        <v>167.45</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>0</v>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="M29" s="4" t="inlineStr">
         <is>
-          <t>0 de 27</t>
+          <t>1 de 27</t>
         </is>
       </c>
       <c r="N29" s="4" t="inlineStr">
@@ -2810,7 +2810,7 @@
         <v>2045.31</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>1670.43</v>
+        <v>1837.88</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>5000</v>
@@ -3070,7 +3070,7 @@
         <v>14727.56</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>1670.43</v>
+        <v>1837.88</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>32000</v>
@@ -3100,7 +3100,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3486,13 +3486,13 @@
         <v>23904.58</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0</v>
+        <v>167.45</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>23904.58</v>
+        <v>23737.13</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0</v>
+        <v>0.007004933782563842</v>
       </c>
     </row>
     <row r="17">
@@ -3553,13 +3553,13 @@
         <v>37500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1670.43</v>
+        <v>1837.88</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>35829.57093005039</v>
+        <v>35662.12093005038</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.04454479889522914</v>
+        <v>0.04901013211781621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-27 17:25:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1250,10 +1250,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>0</v>
+        <v>907.5</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0</v>
+        <v>377.14</v>
       </c>
       <c r="J13" s="2" t="n">
         <v>0</v>
@@ -2211,12 +2211,12 @@
       </c>
       <c r="H29" s="4" t="inlineStr">
         <is>
-          <t>0 de 27</t>
+          <t>1 de 27</t>
         </is>
       </c>
       <c r="I29" s="4" t="inlineStr">
         <is>
-          <t>0 de 27</t>
+          <t>1 de 27</t>
         </is>
       </c>
       <c r="J29" s="4" t="inlineStr">
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>1284.64</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>1000</v>
@@ -3070,7 +3070,7 @@
         <v>14727.56</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>4540.82</v>
+        <v>5825.46</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>32000</v>
@@ -3270,13 +3270,13 @@
         <v>560</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>907.5</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>560</v>
+        <v>-347.5</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>1.620535714285714</v>
       </c>
     </row>
     <row r="8">
@@ -3294,13 +3294,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>377.14</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>625</v>
+        <v>247.86</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0</v>
+        <v>0.603424</v>
       </c>
     </row>
     <row r="9">
@@ -3553,13 +3553,13 @@
         <v>37500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>4540.82</v>
+        <v>5825.46</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>32959.18093005039</v>
+        <v>31674.54093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1210885303301751</v>
+        <v>0.1553455961472205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-27 17:30:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>2702.94</v>
+        <v>4413.66</v>
       </c>
       <c r="M18" s="2" t="n">
         <v>0</v>
@@ -2783,7 +2783,7 @@
         <v>8691.84</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>2702.94</v>
+        <v>4413.66</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>7500</v>
@@ -3070,7 +3070,7 @@
         <v>14727.56</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>5825.46</v>
+        <v>7536.18</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>32000</v>
@@ -3462,13 +3462,13 @@
         <v>1638</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>4373.37</v>
+        <v>6084.09</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-2735.37</v>
+        <v>-4446.09</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>2.669945054945055</v>
+        <v>3.714340659340659</v>
       </c>
     </row>
     <row r="16">
@@ -3553,13 +3553,13 @@
         <v>37500.00093005039</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>5825.46</v>
+        <v>7536.179999999999</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>31674.54093005039</v>
+        <v>29963.82093005039</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1553455961472205</v>
+        <v>0.200964795015803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-08 16:40:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -3285,13 +3285,13 @@
         <v>558.15203605817</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>74.29000000000001</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>558.15203605817</v>
+        <v>483.86203605817</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>0.1330999355026228</v>
       </c>
     </row>
     <row r="5">
@@ -3544,13 +3544,13 @@
         <v>31707.75990313501</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>2503.9</v>
+        <v>2578.19</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>29203.85990313501</v>
+        <v>29129.56990313501</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.07896805096447176</v>
+        <v>0.08131101054997862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-10 16:15:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0</v>
+        <v>212.89</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>0</v>
+        <v>2194.29</v>
       </c>
       <c r="M15" s="2" t="n">
         <v>0</v>
@@ -2246,52 +2246,52 @@
     <row r="30">
       <c r="C30" s="4" t="inlineStr">
         <is>
+          <t>1 de 28</t>
+        </is>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
           <t>0 de 28</t>
         </is>
       </c>
-      <c r="D30" s="4" t="inlineStr">
+      <c r="E30" s="4" t="inlineStr">
         <is>
           <t>0 de 28</t>
         </is>
       </c>
-      <c r="E30" s="4" t="inlineStr">
+      <c r="F30" s="4" t="inlineStr">
         <is>
           <t>0 de 28</t>
         </is>
       </c>
-      <c r="F30" s="4" t="inlineStr">
+      <c r="G30" s="4" t="inlineStr">
         <is>
           <t>0 de 28</t>
         </is>
       </c>
-      <c r="G30" s="4" t="inlineStr">
+      <c r="H30" s="4" t="inlineStr">
+        <is>
+          <t>1 de 28</t>
+        </is>
+      </c>
+      <c r="I30" s="4" t="inlineStr">
+        <is>
+          <t>1 de 28</t>
+        </is>
+      </c>
+      <c r="J30" s="4" t="inlineStr">
         <is>
           <t>0 de 28</t>
         </is>
       </c>
-      <c r="H30" s="4" t="inlineStr">
-        <is>
-          <t>1 de 28</t>
-        </is>
-      </c>
-      <c r="I30" s="4" t="inlineStr">
-        <is>
-          <t>1 de 28</t>
-        </is>
-      </c>
-      <c r="J30" s="4" t="inlineStr">
+      <c r="K30" s="4" t="inlineStr">
         <is>
           <t>0 de 28</t>
         </is>
       </c>
-      <c r="K30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
       <c r="L30" s="4" t="inlineStr">
         <is>
-          <t>2 de 28</t>
+          <t>3 de 28</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0</v>
+        <v>2407.18</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>4000</v>
@@ -3157,7 +3157,7 @@
         <v>7536.18</v>
       </c>
       <c r="F30" s="6" t="n">
-        <v>2503.9</v>
+        <v>4911.08</v>
       </c>
       <c r="G30" s="6" t="n">
         <v>28700</v>
@@ -3185,7 +3185,7 @@
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -3237,13 +3237,13 @@
         <v>1377.24089543035</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>212.89</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1377.24089543035</v>
+        <v>1164.35089543035</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0</v>
+        <v>0.1545771699826541</v>
       </c>
     </row>
     <row r="3">
@@ -3453,13 +3453,13 @@
         <v>5844.44916370549</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>810.25</v>
+        <v>3332.21</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>5034.19916370549</v>
+        <v>2512.23916370549</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0.1386358196135436</v>
+        <v>0.5701495396167184</v>
       </c>
     </row>
     <row r="12">
@@ -3544,13 +3544,13 @@
         <v>31707.75990313501</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>2578.19</v>
+        <v>5313.040000000001</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>29129.56990313501</v>
+        <v>26394.71990313501</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.08131101054997862</v>
+        <v>0.1675627674812402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-10 16:20:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0</v>
+        <v>327.67</v>
       </c>
       <c r="M6" s="2" t="n">
         <v>0</v>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="L30" s="4" t="inlineStr">
         <is>
-          <t>3 de 28</t>
+          <t>4 de 28</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -2519,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>327.67</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>1500</v>
@@ -3157,7 +3157,7 @@
         <v>7536.18</v>
       </c>
       <c r="F30" s="6" t="n">
-        <v>4911.08</v>
+        <v>5238.75</v>
       </c>
       <c r="G30" s="6" t="n">
         <v>28700</v>

</xml_diff>

<commit_message>
Actualización automática 2025-09-10 16:45:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DISALME CIA. LTDA.</t>
+          <t>DELGADO LOOR JORGE ARTURO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
+          <t>DISALME CIA. LTDA.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
+          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GRANIMUNDO S.A.</t>
+          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>725.76</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0</v>
@@ -1351,11 +1351,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LINO TUMBACO VICENTE JAVIER</t>
+          <t>GRANIMUNDO S.A.</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>212.89</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>0</v>
@@ -1382,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>2194.29</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>0</v>
+        <v>725.76</v>
       </c>
       <c r="N15" s="2" t="n">
         <v>0</v>
@@ -1411,11 +1411,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
+          <t>LINO TUMBACO VICENTE JAVIER</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0</v>
+        <v>212.89</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>0</v>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0</v>
+        <v>2194.29</v>
       </c>
       <c r="M16" s="2" t="n">
         <v>0</v>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
+          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>556.8099999999999</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
         <v>0</v>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
+          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>0</v>
+        <v>556.8099999999999</v>
       </c>
       <c r="M18" s="2" t="n">
         <v>0</v>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PAREDES ORTIZ MARIA INES</t>
+          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RENOVA&amp;DISEÑA S.A.</t>
+          <t>PAREDES ORTIZ MARIA INES</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>REYES AGUILERA JESSICA ELIZABETH</t>
+          <t>RENOVA&amp;DISEÑA S.A.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ROCA REYNA PAUL DAVID</t>
+          <t>REYES AGUILERA JESSICA ELIZABETH</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1790,10 +1790,10 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>807</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>160.89</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2" t="n">
         <v>0</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
+          <t>ROCA REYNA PAUL DAVID</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1850,10 +1850,10 @@
         <v>0</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>0</v>
+        <v>807</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>0</v>
+        <v>160.89</v>
       </c>
       <c r="J23" s="2" t="n">
         <v>0</v>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2191,137 +2191,197 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" s="4" t="inlineStr">
-        <is>
-          <t>1 de 28</t>
-        </is>
-      </c>
-      <c r="D30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="E30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="F30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="G30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="H30" s="4" t="inlineStr">
-        <is>
-          <t>1 de 28</t>
-        </is>
-      </c>
-      <c r="I30" s="4" t="inlineStr">
-        <is>
-          <t>1 de 28</t>
-        </is>
-      </c>
-      <c r="J30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="K30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="L30" s="4" t="inlineStr">
-        <is>
-          <t>4 de 28</t>
-        </is>
-      </c>
-      <c r="M30" s="4" t="inlineStr">
-        <is>
-          <t>1 de 28</t>
-        </is>
-      </c>
-      <c r="N30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="O30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="P30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="Q30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
-        </is>
-      </c>
-      <c r="R30" s="4" t="inlineStr">
-        <is>
-          <t>0 de 28</t>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="4" t="inlineStr">
+        <is>
+          <t>1 de 29</t>
+        </is>
+      </c>
+      <c r="D31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="F31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="H31" s="4" t="inlineStr">
+        <is>
+          <t>1 de 29</t>
+        </is>
+      </c>
+      <c r="I31" s="4" t="inlineStr">
+        <is>
+          <t>1 de 29</t>
+        </is>
+      </c>
+      <c r="J31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="K31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="L31" s="4" t="inlineStr">
+        <is>
+          <t>4 de 29</t>
+        </is>
+      </c>
+      <c r="M31" s="4" t="inlineStr">
+        <is>
+          <t>1 de 29</t>
+        </is>
+      </c>
+      <c r="N31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="O31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="P31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="Q31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
+        </is>
+      </c>
+      <c r="R31" s="4" t="inlineStr">
+        <is>
+          <t>0 de 29</t>
         </is>
       </c>
     </row>
@@ -2336,7 +2396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2641,7 +2701,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DISALME CIA. LTDA.</t>
+          <t>DELGADO LOOR JORGE ARTURO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -2668,7 +2728,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
+          <t>DISALME CIA. LTDA.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -2695,7 +2755,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
+          <t>FERRETERIA UNIDA ZAMBRANO FERRUZAM CIA. LTDA.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -2722,23 +2782,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GRANIMUNDO S.A.</t>
+          <t>FREILE FERRIN FRECIA NOEMI LOURDE</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>738.66</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>1284.64</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>725.76</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2749,23 +2809,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LINO TUMBACO VICENTE JAVIER</t>
+          <t>GRANIMUNDO S.A.</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>1473.73</v>
+        <v>738.66</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>3990.41</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0</v>
+        <v>1284.64</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>2407.18</v>
+        <v>725.76</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="16">
@@ -2776,23 +2836,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
+          <t>LINO TUMBACO VICENTE JAVIER</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0</v>
+        <v>1473.73</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0</v>
+        <v>3990.41</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>2407.18</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="17">
@@ -2803,7 +2863,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
+          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -2816,10 +2876,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>556.8099999999999</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2830,11 +2890,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
+          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>9556.26</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>0</v>
@@ -2843,10 +2903,10 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>556.8099999999999</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>3500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="19">
@@ -2857,23 +2917,23 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PAREDES ORTIZ MARIA INES</t>
+          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>64.81999999999999</v>
+        <v>9556.26</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>8691.84</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>4413.66</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>8000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="20">
@@ -2884,23 +2944,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RENOVA&amp;DISEÑA S.A.</t>
+          <t>PAREDES ORTIZ MARIA INES</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>411.7</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2045.31</v>
+        <v>8691.84</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>1837.88</v>
+        <v>4413.66</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>5000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="21">
@@ -2911,23 +2971,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>REYES AGUILERA JESSICA ELIZABETH</t>
+          <t>RENOVA&amp;DISEÑA S.A.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0</v>
+        <v>411.7</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0</v>
+        <v>2045.31</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0</v>
+        <v>1837.88</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="22">
@@ -2938,11 +2998,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ROCA REYNA PAUL DAVID</t>
+          <t>REYES AGUILERA JESSICA ELIZABETH</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>3225.33</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>0</v>
@@ -2951,10 +3011,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>967.89</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2965,11 +3025,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
+          <t>ROCA REYNA PAUL DAVID</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0</v>
+        <v>3225.33</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>0</v>
@@ -2978,10 +3038,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0</v>
+        <v>967.89</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="24">
@@ -2992,7 +3052,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -3019,7 +3079,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -3046,7 +3106,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -3073,7 +3133,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -3100,7 +3160,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -3127,39 +3187,66 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" s="6" t="n">
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="6" t="n">
         <v>15470.5</v>
       </c>
-      <c r="D30" s="6" t="n">
+      <c r="D31" s="6" t="n">
         <v>14727.56</v>
       </c>
-      <c r="E30" s="6" t="n">
+      <c r="E31" s="6" t="n">
         <v>7536.18</v>
       </c>
-      <c r="F30" s="6" t="n">
+      <c r="F31" s="6" t="n">
         <v>5238.75</v>
       </c>
-      <c r="G30" s="6" t="n">
+      <c r="G31" s="6" t="n">
         <v>28700</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 16:45:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>725.76</v>
+        <v>1451.52</v>
       </c>
       <c r="N15" s="2" t="n">
         <v>0</v>
@@ -2822,7 +2822,7 @@
         <v>1284.64</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>725.76</v>
+        <v>1451.52</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>2000</v>
@@ -3244,7 +3244,7 @@
         <v>7536.18</v>
       </c>
       <c r="F31" s="6" t="n">
-        <v>5517.16</v>
+        <v>6242.92</v>
       </c>
       <c r="G31" s="6" t="n">
         <v>28700</v>
@@ -3564,13 +3564,13 @@
         <v>17675.3486842162</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>725.76</v>
+        <v>1451.52</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>16949.5886842162</v>
+        <v>16223.8286842162</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.04106057611457996</v>
+        <v>0.08212115222915993</v>
       </c>
     </row>
     <row r="13">
@@ -3631,13 +3631,13 @@
         <v>31707.75990313501</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>5591.450000000001</v>
+        <v>6317.210000000001</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>26116.30990313501</v>
+        <v>25390.54990313501</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.1763432679281504</v>
+        <v>0.1992323021020292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-15 09:54:22
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GRANIMUNDO S.A.</t>
+          <t>GONZALEZ CARDENAS ERNESTO PAOLO</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>1451.52</v>
+        <v>0</v>
       </c>
       <c r="N15" s="2" t="n">
         <v>0</v>
@@ -1411,11 +1411,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LINO TUMBACO VICENTE JAVIER</t>
+          <t>GRANIMUNDO S.A.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>212.89</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>0</v>
@@ -1442,10 +1442,10 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>2194.29</v>
+        <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0</v>
+        <v>1451.52</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -1471,11 +1471,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
+          <t>LINO TUMBACO VICENTE JAVIER</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>212.89</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>0</v>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>0</v>
+        <v>2194.29</v>
       </c>
       <c r="M17" s="2" t="n">
         <v>0</v>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
+          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>835.22</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2" t="n">
         <v>0</v>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
+          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>0</v>
+        <v>835.22</v>
       </c>
       <c r="M19" s="2" t="n">
         <v>0</v>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PAREDES ORTIZ MARIA INES</t>
+          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RENOVA&amp;DISEÑA S.A.</t>
+          <t>PAREDES ORTIZ MARIA INES</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>REYES AGUILERA JESSICA ELIZABETH</t>
+          <t>RENOVA&amp;DISEÑA S.A.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ROCA REYNA PAUL DAVID</t>
+          <t>REYES AGUILERA JESSICA ELIZABETH</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1850,10 +1850,10 @@
         <v>0</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>807</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>160.89</v>
+        <v>0</v>
       </c>
       <c r="J23" s="2" t="n">
         <v>0</v>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
+          <t>ROCA REYNA PAUL DAVID</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1910,10 +1910,10 @@
         <v>0</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>0</v>
+        <v>807</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>0</v>
+        <v>160.89</v>
       </c>
       <c r="J24" s="2" t="n">
         <v>0</v>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2251,137 +2251,197 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" s="4" t="inlineStr">
-        <is>
-          <t>1 de 29</t>
-        </is>
-      </c>
-      <c r="D31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="E31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="F31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="G31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="H31" s="4" t="inlineStr">
-        <is>
-          <t>1 de 29</t>
-        </is>
-      </c>
-      <c r="I31" s="4" t="inlineStr">
-        <is>
-          <t>1 de 29</t>
-        </is>
-      </c>
-      <c r="J31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="K31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="L31" s="4" t="inlineStr">
-        <is>
-          <t>4 de 29</t>
-        </is>
-      </c>
-      <c r="M31" s="4" t="inlineStr">
-        <is>
-          <t>1 de 29</t>
-        </is>
-      </c>
-      <c r="N31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="O31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="P31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="Q31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
-        </is>
-      </c>
-      <c r="R31" s="4" t="inlineStr">
-        <is>
-          <t>0 de 29</t>
+      <c r="C31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>1 de 30</t>
+        </is>
+      </c>
+      <c r="D32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="H32" s="4" t="inlineStr">
+        <is>
+          <t>1 de 30</t>
+        </is>
+      </c>
+      <c r="I32" s="4" t="inlineStr">
+        <is>
+          <t>1 de 30</t>
+        </is>
+      </c>
+      <c r="J32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="K32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="L32" s="4" t="inlineStr">
+        <is>
+          <t>4 de 30</t>
+        </is>
+      </c>
+      <c r="M32" s="4" t="inlineStr">
+        <is>
+          <t>1 de 30</t>
+        </is>
+      </c>
+      <c r="N32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="O32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="P32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="Q32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
+        </is>
+      </c>
+      <c r="R32" s="4" t="inlineStr">
+        <is>
+          <t>0 de 30</t>
         </is>
       </c>
     </row>
@@ -2396,7 +2456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2809,23 +2869,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GRANIMUNDO S.A.</t>
+          <t>GONZALEZ CARDENAS ERNESTO PAOLO</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>738.66</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1284.64</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>1451.52</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2836,23 +2896,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LINO TUMBACO VICENTE JAVIER</t>
+          <t>GRANIMUNDO S.A.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>1473.73</v>
+        <v>738.66</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>3990.41</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0</v>
+        <v>1284.64</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>2407.18</v>
+        <v>1451.52</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17">
@@ -2863,23 +2923,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
+          <t>LINO TUMBACO VICENTE JAVIER</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>1473.73</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>3990.41</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0</v>
+        <v>2407.18</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="18">
@@ -2890,7 +2950,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
+          <t>MANABITA DE REPUESTOS MANARECO C LTDA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -2903,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>835.22</v>
+        <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2917,11 +2977,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
+          <t>MATERIALES PARA DECORACION DECORCASA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>9556.26</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>0</v>
@@ -2930,10 +2990,10 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>835.22</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>3500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="20">
@@ -2944,23 +3004,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PAREDES ORTIZ MARIA INES</t>
+          <t>MOREIRA MOREIRA PATRICIO IGNACIO</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>64.81999999999999</v>
+        <v>9556.26</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>8691.84</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>4413.66</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>8000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="21">
@@ -2971,23 +3031,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RENOVA&amp;DISEÑA S.A.</t>
+          <t>PAREDES ORTIZ MARIA INES</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>411.7</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>2045.31</v>
+        <v>8691.84</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>1837.88</v>
+        <v>4413.66</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>5000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="22">
@@ -2998,23 +3058,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>REYES AGUILERA JESSICA ELIZABETH</t>
+          <t>RENOVA&amp;DISEÑA S.A.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0</v>
+        <v>411.7</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0</v>
+        <v>2045.31</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0</v>
+        <v>1837.88</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="23">
@@ -3025,11 +3085,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ROCA REYNA PAUL DAVID</t>
+          <t>REYES AGUILERA JESSICA ELIZABETH</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>3225.33</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>0</v>
@@ -3038,10 +3098,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>967.89</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -3052,11 +3112,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
+          <t>ROCA REYNA PAUL DAVID</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0</v>
+        <v>3225.33</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>0</v>
@@ -3065,10 +3125,10 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>0</v>
+        <v>967.89</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="25">
@@ -3079,7 +3139,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SUMBA GARCIA MARCOS ANTONIO</t>
+          <t>SOLORZANO BRAVO TERESA CONCEPCION</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -3106,7 +3166,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
+          <t>SUMBA GARCIA MARCOS ANTONIO</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -3133,7 +3193,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
+          <t>TUTIVEN PAREDES MARCIA PIEDAD</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -3160,7 +3220,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>VERA ARCE MARIA ISABEL</t>
+          <t>VACA CANCHINGRE FATIMA YAQUELINE</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -3187,7 +3247,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+          <t>VERA ARCE MARIA ISABEL</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -3214,39 +3274,66 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>ZAMBRANO FERNANDEZ JOSE LUIS</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>ZAMBRANO REYNA JOSE ALEJANDRO</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" s="6" t="n">
+      <c r="C31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="6" t="n">
         <v>15470.5</v>
       </c>
-      <c r="D31" s="6" t="n">
+      <c r="D32" s="6" t="n">
         <v>14727.56</v>
       </c>
-      <c r="E31" s="6" t="n">
+      <c r="E32" s="6" t="n">
         <v>7536.18</v>
       </c>
-      <c r="F31" s="6" t="n">
+      <c r="F32" s="6" t="n">
         <v>6242.92</v>
       </c>
-      <c r="G31" s="6" t="n">
+      <c r="G32" s="6" t="n">
         <v>28700</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-24 09:45:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>1451.52</v>
+        <v>1463.58</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -2909,7 +2909,7 @@
         <v>1284.64</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>1451.52</v>
+        <v>1463.58</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>2000</v>
@@ -3331,7 +3331,7 @@
         <v>7536.18</v>
       </c>
       <c r="F32" s="6" t="n">
-        <v>9589.41</v>
+        <v>9601.469999999999</v>
       </c>
       <c r="G32" s="6" t="n">
         <v>28700</v>
@@ -3361,7 +3361,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3651,13 +3651,13 @@
         <v>17675.3486842162</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>1451.52</v>
+        <v>1463.58</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>16223.8286842162</v>
+        <v>16211.7686842162</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.08212115222915993</v>
+        <v>0.0828034584294766</v>
       </c>
     </row>
     <row r="13">
@@ -3718,13 +3718,13 @@
         <v>31707.75990313501</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>9663.700000000001</v>
+        <v>9675.76</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>22044.05990313501</v>
+        <v>22031.99990313501</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.3047739742423284</v>
+        <v>0.3051543227764677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-03 17:30:08
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1898,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>0</v>
+        <v>1391.04</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="D32" s="4" t="inlineStr">
         <is>
-          <t>0 de 30</t>
+          <t>1 de 30</t>
         </is>
       </c>
       <c r="E32" s="4" t="inlineStr">
@@ -3125,7 +3125,7 @@
         <v>2868.69</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>0</v>
+        <v>1391.04</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>3000</v>
@@ -3331,7 +3331,7 @@
         <v>9784.639999999999</v>
       </c>
       <c r="F32" s="6" t="n">
-        <v>0</v>
+        <v>1391.04</v>
       </c>
       <c r="G32" s="6" t="n">
         <v>28700</v>

</xml_diff>

<commit_message>
Actualización automática 2025-10-08 17:30:10
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>86.5</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>0</v>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="D32" s="4" t="inlineStr">
         <is>
-          <t>2 de 30</t>
+          <t>3 de 30</t>
         </is>
       </c>
       <c r="E32" s="4" t="inlineStr">
@@ -2639,7 +2639,7 @@
         <v>655.34</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>86.5</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
@@ -3331,7 +3331,7 @@
         <v>9784.639999999999</v>
       </c>
       <c r="F32" s="6" t="n">
-        <v>1644.48</v>
+        <v>1730.98</v>
       </c>
       <c r="G32" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-10-28 12:30:09
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0</v>
+        <v>1382.33</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="M32" s="4" t="inlineStr">
         <is>
-          <t>0 de 30</t>
+          <t>1 de 30</t>
         </is>
       </c>
       <c r="N32" s="4" t="inlineStr">
@@ -2909,7 +2909,7 @@
         <v>1463.58</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>1382.33</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>0</v>
@@ -3331,7 +3331,7 @@
         <v>9784.639999999999</v>
       </c>
       <c r="F32" s="6" t="n">
-        <v>2454.34</v>
+        <v>3836.67</v>
       </c>
       <c r="G32" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-11-05 16:30:07
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>489.11</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="M32" s="4" t="inlineStr">
         <is>
-          <t>0 de 30</t>
+          <t>1 de 30</t>
         </is>
       </c>
       <c r="N32" s="4" t="inlineStr">
@@ -2558,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>489.11</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -3331,7 +3331,7 @@
         <v>3836.67</v>
       </c>
       <c r="F32" s="6" t="n">
-        <v>0</v>
+        <v>489.11</v>
       </c>
       <c r="G32" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-11-11 16:30:07
</commit_message>
<xml_diff>
--- a/data/LOZANO MOLINA TITO.xlsx
+++ b/data/LOZANO MOLINA TITO.xlsx
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>0</v>
+        <v>5511.6</v>
       </c>
       <c r="M21" s="2" t="n">
         <v>0</v>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="L32" s="4" t="inlineStr">
         <is>
-          <t>0 de 30</t>
+          <t>1 de 30</t>
         </is>
       </c>
       <c r="M32" s="4" t="inlineStr">
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0</v>
+        <v>5511.6</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>0</v>
@@ -3331,7 +3331,7 @@
         <v>3836.67</v>
       </c>
       <c r="F32" s="6" t="n">
-        <v>489.11</v>
+        <v>6000.71</v>
       </c>
       <c r="G32" s="6" t="n">
         <v>0</v>

</xml_diff>